<commit_message>
2021-05-12 첨부파일 샘플 commit
</commit_message>
<xml_diff>
--- a/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
+++ b/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\모집인등록테스트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCA8DD2F-76E6-4E1E-9CA3-FD0FF7CD10BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200454A6-6DE6-4B51-8BB9-E9F2ABC1B551}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E1223E6-BF72-441D-977A-03078155171A}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>구분</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -139,6 +139,14 @@
 매출채권 매입 = 5
 지급보증 = 6
 기타 대출성상품 = 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>상세주소</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>용산구 한남동 00-00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -539,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DC9980-449E-431A-AF95-CC100EDA729F}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -550,14 +558,14 @@
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.296875" customWidth="1"/>
-    <col min="6" max="6" width="25.19921875" customWidth="1"/>
-    <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.8984375" customWidth="1"/>
-    <col min="10" max="13" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="28.296875" customWidth="1"/>
+    <col min="7" max="7" width="25.19921875" customWidth="1"/>
+    <col min="9" max="9" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.8984375" customWidth="1"/>
+    <col min="11" max="14" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -574,31 +582,34 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="295.8" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:14" ht="295.8" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
         <v>20</v>
       </c>
@@ -614,17 +625,15 @@
       <c r="E2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
@@ -635,8 +644,11 @@
       <c r="M2" t="s">
         <v>18</v>
       </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>1</v>
       </c>
@@ -652,22 +664,25 @@
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>1234123412</v>
       </c>
-      <c r="J3" s="2">
+      <c r="K3" s="2">
         <v>44326</v>
       </c>
-      <c r="K3" s="2">
+      <c r="L3" s="2">
         <v>44328</v>
       </c>
-      <c r="L3" s="2">
+      <c r="M3" s="2">
         <v>44330</v>
       </c>
-      <c r="M3" s="2">
+      <c r="N3" s="2">
         <v>44369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021-05-13 문구수정 및 vali 변경 commit
</commit_message>
<xml_diff>
--- a/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
+++ b/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\모집인등록테스트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AD0AA47-97A1-4D21-8482-953E09E474EB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD989B74-FDF5-4F73-A59B-CEBF3EDE097D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E1223E6-BF72-441D-977A-03078155171A}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E1223E6-BF72-441D-977A-03078155171A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,94 +25,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
-  <si>
-    <t>구분</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>성명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주민등록번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>휴대폰번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>주소</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>금융상품유형</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>법인명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>법인등록번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>교육이수번호/인증서번호</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경력시작일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>경력종료일</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>계약일자</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위탁예정기간</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신동환</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>010-3167-2126</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>000000-0000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>880131-0000000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>010-0000-0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>YYYY-MM-DD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0000000000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>신규 = 1
+    <t>구분
+신규 = 1
 경력 = 2</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>서울 = 1
+    <t>주민등록번호
+000000-0000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>휴대폰번호
+000-0000-0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>주소
+서울 = 1
 경기 = 2
 충청북도 = 3
 충청남도 = 4
@@ -132,13 +80,48 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>대출 = 1
+    <t>금융상품유형
+대출 = 1
 시설대여 및 연불판매 = 2
 할부 = 3
 어음할인 = 4
 매출채권 매입 = 5
 지급보증 = 6
 기타 대출성상품 = 7</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>법인등록번호
+000000-0000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>교육이수번호/인증서번호
+0000000000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경력시작일
+YYYY-MM-DD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>경력종료일
+YYYY-MM-DD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>계약일자
+YYYY-MM-DD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>위탁예정기간
+YYYY-MM-DD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍길동</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -206,7 +189,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -216,14 +199,11 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -539,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DC9980-449E-431A-AF95-CC100EDA729F}">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -553,121 +533,83 @@
     <col min="5" max="5" width="28.296875" customWidth="1"/>
     <col min="6" max="6" width="25.19921875" customWidth="1"/>
     <col min="8" max="8" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.8984375" customWidth="1"/>
+    <col min="9" max="9" width="22.8984375" customWidth="1"/>
     <col min="10" max="13" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" s="1" customFormat="1" ht="313.2" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="H1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="295.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>18</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A3">
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
-      <c r="I3">
+      <c r="I2">
         <v>1234123412</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J2" s="2">
         <v>44326</v>
       </c>
-      <c r="K3" s="2">
+      <c r="K2" s="2">
         <v>44328</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L2" s="2">
         <v>44330</v>
       </c>
-      <c r="M3" s="2">
+      <c r="M2" s="2">
         <v>44369</v>
       </c>
     </row>

</xml_diff>

<commit_message>
2021-05-13 샘플다운로드 문서 commit
</commit_message>
<xml_diff>
--- a/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
+++ b/src/main/resources/static/sample/모집인등록_개인_샘플.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a\Desktop\모집인등록테스트\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD989B74-FDF5-4F73-A59B-CEBF3EDE097D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1173BDB-31FD-44ED-BFE8-4EA388933CD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{8E1223E6-BF72-441D-977A-03078155171A}"/>
   </bookViews>
@@ -24,8 +24,795 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>a</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{91DFEFCA-DEB2-4DD4-BD8A-4D5055EFD4C3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>신규</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>경력</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{5D1D51BB-F709-44B6-A546-F8969FCF4507}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>000000-0000000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{7A94D858-3FEE-4730-8118-070B29082985}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>000-0000-0000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{F0B31075-CD8A-4F6D-9588-DA3CA910932B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>서울</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>경기</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>충청북도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 3
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>충청남도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>강원도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>경상북도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 6
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>경상남도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 7
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>전라북도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 8
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>전라남도</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 9
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>인천</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 10
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>세종</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 11
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대전</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 12
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대구</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 13
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>울산</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 14
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>광주</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 15
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>부산</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 16
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>제주</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 17</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{A6FDD5DA-CBAC-40BA-BC0F-22DE3367E88B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대출</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 1
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>시설대여</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>및</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>연불판매</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 2
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>할부</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 3
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>어음할인</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 4
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>매출채권</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>매입</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 5
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>지급보증</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 6
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>기타</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> </t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="돋움"/>
+            <family val="3"/>
+            <charset val="129"/>
+          </rPr>
+          <t>대출성상품</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> = 7</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{C7ED3F6D-4891-4FAF-A704-D825DB817AFB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>000000-0000000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{571DC4E6-3BC8-406C-84BC-C733A622FE0A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>0000000000</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{038AE3B3-B4C0-4D80-95AF-7400DA5FF847}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{63431FC7-91F5-4498-AD32-94A2B8F910FC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{263D8AD0-F07A-4989-8C2D-E66F5849401B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{DB27BFB9-D1FD-4100-8C59-63FF4192AA6F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>YYYY-MM-DD</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>성명</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,93 +822,47 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>010-3167-2126</t>
+    <t>주소</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>880131-0000000</t>
+    <t>금융상품유형</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>구분
-신규 = 1
-경력 = 2</t>
+    <t>주민등록번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주민등록번호
-000000-0000000</t>
+    <t>구분</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>휴대폰번호
-000-0000-0000</t>
+    <t>휴대폰번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>주소
-서울 = 1
-경기 = 2
-충청북도 = 3
-충청남도 = 4
-강원도 = 5
-경상북도 = 6
-경상남도 = 7
-전라북도 = 8
-전라남도 = 9
-인천 = 10
-세종 = 11
-대전 = 12
-대구 = 13
-울산 = 14
-광주 = 15
-부산 = 16
-제주 = 17</t>
+    <t>법인등록번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>금융상품유형
-대출 = 1
-시설대여 및 연불판매 = 2
-할부 = 3
-어음할인 = 4
-매출채권 매입 = 5
-지급보증 = 6
-기타 대출성상품 = 7</t>
+    <t>교육이수번호/인증서번호</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>법인등록번호
-000000-0000000</t>
+    <t>경력시작일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>교육이수번호/인증서번호
-0000000000</t>
+    <t>경력종료일</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>경력시작일
-YYYY-MM-DD</t>
+    <t>계약일자</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>경력종료일
-YYYY-MM-DD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>계약일자
-YYYY-MM-DD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>위탁예정기간
-YYYY-MM-DD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>홍길동</t>
+    <t>위탁예정기간</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -129,7 +870,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +885,21 @@
       <family val="2"/>
       <charset val="129"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="돋움"/>
+      <family val="3"/>
+      <charset val="129"/>
     </font>
   </fonts>
   <fills count="3">
@@ -189,15 +945,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -518,11 +1271,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DC9980-449E-431A-AF95-CC100EDA729F}">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C7DC9980-449E-431A-AF95-CC100EDA729F}">
+  <dimension ref="A1:M1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -537,85 +1290,51 @@
     <col min="10" max="13" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" ht="313.2" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>1234123412</v>
-      </c>
-      <c r="J2" s="2">
-        <v>44326</v>
-      </c>
-      <c r="K2" s="2">
-        <v>44328</v>
-      </c>
-      <c r="L2" s="2">
-        <v>44330</v>
-      </c>
-      <c r="M2" s="2">
-        <v>44369</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>